<commit_message>
reset password & bulk regis
</commit_message>
<xml_diff>
--- a/public/assets/excel/register.xlsx
+++ b/public/assets/excel/register.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF1EB55-2528-4F99-98DD-20410E432204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E84BB1-51CD-463C-9798-8EF31CF9DB84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0DB44E57-BC8F-4CB9-BB7C-CB79F8B9A592}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>nip</t>
   </si>
@@ -45,9 +45,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>BKN</t>
-  </si>
-  <si>
     <t>Analis SDM Aparatur</t>
   </si>
   <si>
@@ -63,46 +60,34 @@
     <t>jenjang</t>
   </si>
   <si>
-    <t>Randi, S.Kom.</t>
-  </si>
-  <si>
-    <t>Dhanu, S.E.</t>
-  </si>
-  <si>
-    <t>Pranata SDM Aparatur</t>
-  </si>
-  <si>
-    <t>Ahli Pertama</t>
-  </si>
-  <si>
-    <t>Mahir</t>
-  </si>
-  <si>
-    <t>199500112022031003</t>
-  </si>
-  <si>
-    <t>199501119920310051</t>
-  </si>
-  <si>
-    <t>randi@gmail.com1</t>
-  </si>
-  <si>
-    <t>dhanu@gmail.com1</t>
-  </si>
-  <si>
-    <t>081999099901</t>
-  </si>
-  <si>
-    <t>088889999901</t>
-  </si>
-  <si>
     <t>paid</t>
   </si>
   <si>
-    <t>C:\Users\user\Documents\proposal.pdf</t>
-  </si>
-  <si>
     <t>document_jab</t>
+  </si>
+  <si>
+    <t>documents/blank.pdf</t>
+  </si>
+  <si>
+    <t>198409142003121002</t>
+  </si>
+  <si>
+    <t>ASEP RIYANTO, S.STP.</t>
+  </si>
+  <si>
+    <t>asriy.oppof9@gmail.com</t>
+  </si>
+  <si>
+    <t>'082316840508</t>
+  </si>
+  <si>
+    <t>Pemerintah Provinsi Jawa Barat</t>
+  </si>
+  <si>
+    <t>Madya</t>
+  </si>
+  <si>
+    <t>documents/jabarkolektif9.jpeg</t>
   </si>
 </sst>
 </file>
@@ -469,21 +454,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB59973-933E-4EF1-BF71-7820EF3D657B}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -497,87 +484,54 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{9123145A-DFDB-4A72-949C-24995EAE49D7}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{8E076F05-A84C-4EB0-B489-109C37A19920}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>